<commit_message>
CIERRE 11 NOV 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 10  OCTUBRE 2021/BALANCE    ZAVALETA   OCTUBRE   2021.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 10  OCTUBRE 2021/BALANCE    ZAVALETA   OCTUBRE   2021.xlsx
@@ -145,9 +145,6 @@
     <t>INVENTARIO FINAL</t>
   </si>
   <si>
-    <t>GANANCIA</t>
-  </si>
-  <si>
     <t>FECHA</t>
   </si>
   <si>
@@ -398,6 +395,9 @@
   </si>
   <si>
     <t>Devoluciones</t>
+  </si>
+  <si>
+    <t>PERDIDA</t>
   </si>
 </sst>
 </file>
@@ -412,7 +412,7 @@
     <numFmt numFmtId="167" formatCode="[$$-80A]#,##0.00;\-[$$-80A]#,##0.00"/>
     <numFmt numFmtId="168" formatCode="[$-C0A]d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="47" x14ac:knownFonts="1">
+  <fonts count="48" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -785,8 +785,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -847,8 +855,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="57">
+  <borders count="61">
     <border>
       <left/>
       <right/>
@@ -1558,12 +1572,56 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="264">
+  <cellXfs count="275">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1967,126 +2025,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="44" fontId="44" fillId="6" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="3" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="3" borderId="51" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="3" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="50" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="43" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="43" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="15" fontId="2" fillId="10" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2128,6 +2066,141 @@
     <xf numFmtId="44" fontId="3" fillId="9" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="9" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="39" fillId="11" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="39" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="13" fillId="6" borderId="58" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="59" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="56" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="60" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="47" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="6" borderId="51" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="6" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="50" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="43" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="43" fillId="6" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -2848,17 +2921,17 @@
   </sheetPr>
   <dimension ref="A1:S80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="K62" sqref="K62"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.28515625" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" style="97" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" style="4" customWidth="1"/>
     <col min="7" max="7" width="1.85546875" customWidth="1"/>
     <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.7109375" style="4" customWidth="1"/>
@@ -2867,30 +2940,30 @@
     <col min="12" max="12" width="14.5703125" style="3" customWidth="1"/>
     <col min="13" max="13" width="15.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" customWidth="1"/>
     <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="18.140625" style="2" customWidth="1"/>
     <col min="18" max="18" width="15.28515625" style="176" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="205"/>
-      <c r="C1" s="207" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="208"/>
-      <c r="E1" s="208"/>
-      <c r="F1" s="208"/>
-      <c r="G1" s="208"/>
-      <c r="H1" s="208"/>
-      <c r="I1" s="208"/>
-      <c r="J1" s="208"/>
-      <c r="K1" s="208"/>
-      <c r="L1" s="208"/>
-      <c r="M1" s="208"/>
-    </row>
-    <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="206"/>
+    <row r="1" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B1" s="235"/>
+      <c r="C1" s="237" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="238"/>
+      <c r="E1" s="238"/>
+      <c r="F1" s="238"/>
+      <c r="G1" s="238"/>
+      <c r="H1" s="238"/>
+      <c r="I1" s="238"/>
+      <c r="J1" s="238"/>
+      <c r="K1" s="238"/>
+      <c r="L1" s="238"/>
+      <c r="M1" s="238"/>
+    </row>
+    <row r="2" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="236"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -2899,23 +2972,23 @@
       <c r="M2" s="6"/>
       <c r="N2" s="9"/>
     </row>
-    <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="209" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="210"/>
+    <row r="3" spans="1:19" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="239" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="240"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="211" t="s">
-        <v>31</v>
-      </c>
-      <c r="I3" s="211"/>
+      <c r="H3" s="241" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" s="241"/>
       <c r="K3" s="178"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
     </row>
-    <row r="4" spans="1:18" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
         <v>1</v>
       </c>
@@ -2924,14 +2997,14 @@
         <v>0</v>
       </c>
       <c r="D4" s="18"/>
-      <c r="E4" s="212" t="s">
+      <c r="E4" s="242" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="213"/>
-      <c r="H4" s="214" t="s">
+      <c r="F4" s="243"/>
+      <c r="H4" s="244" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="215"/>
+      <c r="I4" s="245"/>
       <c r="J4" s="19"/>
       <c r="K4" s="179"/>
       <c r="L4" s="20"/>
@@ -2941,12 +3014,12 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="221" t="s">
+      <c r="P4" s="251" t="s">
         <v>6</v>
       </c>
-      <c r="Q4" s="222"/>
-    </row>
-    <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q4" s="252"/>
+    </row>
+    <row r="5" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
         <v>7</v>
       </c>
@@ -2971,7 +3044,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K5" s="31"/>
       <c r="L5" s="9"/>
@@ -2992,7 +3065,7 @@
       </c>
       <c r="R5" s="31"/>
     </row>
-    <row r="6" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="23"/>
       <c r="B6" s="24">
         <v>44489</v>
@@ -3018,7 +3091,7 @@
         <v>44489</v>
       </c>
       <c r="K6" s="38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L6" s="39">
         <v>3000</v>
@@ -3034,15 +3107,18 @@
         <f t="shared" ref="P6:P32" si="0">N6+M6+L6+I6+C6</f>
         <v>20860</v>
       </c>
-      <c r="Q6" s="258">
+      <c r="Q6" s="218">
         <f t="shared" ref="Q6:Q38" si="1">P6-F6</f>
         <v>-2677</v>
       </c>
-      <c r="R6" s="256" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R6" s="216" t="s">
+        <v>32</v>
+      </c>
+      <c r="S6" s="147">
+        <v>44489</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="23"/>
       <c r="B7" s="24">
         <v>44490</v>
@@ -3068,7 +3144,7 @@
         <v>44489</v>
       </c>
       <c r="K7" s="38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L7" s="39">
         <v>3000</v>
@@ -3079,22 +3155,25 @@
       <c r="N7" s="33">
         <v>8843</v>
       </c>
-      <c r="O7" s="255" t="s">
-        <v>36</v>
+      <c r="O7" s="215" t="s">
+        <v>35</v>
       </c>
       <c r="P7" s="69">
         <f t="shared" si="0"/>
         <v>27818</v>
       </c>
-      <c r="Q7" s="259">
+      <c r="Q7" s="219">
         <f t="shared" si="1"/>
         <v>2027</v>
       </c>
-      <c r="R7" s="257" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R7" s="217" t="s">
+        <v>43</v>
+      </c>
+      <c r="S7" s="147">
+        <v>44490</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="23"/>
       <c r="B8" s="24">
         <v>44491</v>
@@ -3103,7 +3182,7 @@
         <v>206.5</v>
       </c>
       <c r="D8" s="42" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E8" s="27">
         <v>44491</v>
@@ -3122,7 +3201,7 @@
         <v>44491</v>
       </c>
       <c r="K8" s="38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L8" s="39">
         <v>3300</v>
@@ -3138,15 +3217,18 @@
         <f t="shared" si="0"/>
         <v>25278.5</v>
       </c>
-      <c r="Q8" s="260">
+      <c r="Q8" s="220">
         <f t="shared" si="1"/>
         <v>-3392.5</v>
       </c>
-      <c r="R8" s="256" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R8" s="216" t="s">
+        <v>32</v>
+      </c>
+      <c r="S8" s="147">
+        <v>44491</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="23"/>
       <c r="B9" s="24">
         <v>44492</v>
@@ -3172,7 +3254,7 @@
         <v>44492</v>
       </c>
       <c r="K9" s="193" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L9" s="194">
         <v>1800</v>
@@ -3189,14 +3271,17 @@
         <f>N9+M9+L9+I9+C9</f>
         <v>36624.5</v>
       </c>
-      <c r="Q9" s="261" t="s">
-        <v>59</v>
-      </c>
-      <c r="R9" s="257" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q9" s="221" t="s">
+        <v>58</v>
+      </c>
+      <c r="R9" s="217" t="s">
+        <v>38</v>
+      </c>
+      <c r="S9" s="147">
+        <v>44492</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="23"/>
       <c r="B10" s="24">
         <v>44493</v>
@@ -3205,7 +3290,7 @@
         <v>326</v>
       </c>
       <c r="D10" s="40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E10" s="27">
         <v>44493</v>
@@ -3224,7 +3309,7 @@
         <v>44493</v>
       </c>
       <c r="K10" s="180" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L10" s="45">
         <v>7500</v>
@@ -3240,15 +3325,18 @@
         <f t="shared" ref="P10:P13" si="2">N10+M10+L10+I10+C10</f>
         <v>26298</v>
       </c>
-      <c r="Q10" s="260">
+      <c r="Q10" s="220">
         <f t="shared" si="1"/>
         <v>-1776</v>
       </c>
-      <c r="R10" s="256" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R10" s="216" t="s">
+        <v>32</v>
+      </c>
+      <c r="S10" s="147">
+        <v>44493</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="23"/>
       <c r="B11" s="24">
         <v>44494</v>
@@ -3258,7 +3346,7 @@
         <v>21328</v>
       </c>
       <c r="D11" s="35" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E11" s="27">
         <v>44494</v>
@@ -3287,15 +3375,18 @@
         <f t="shared" si="2"/>
         <v>28522</v>
       </c>
-      <c r="Q11" s="262">
+      <c r="Q11" s="222">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R11" s="38" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+      <c r="S11" s="147">
+        <v>44494</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="23"/>
       <c r="B12" s="24">
         <v>44495</v>
@@ -3305,7 +3396,7 @@
         <v>14061</v>
       </c>
       <c r="D12" s="35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E12" s="27">
         <v>44495</v>
@@ -3334,15 +3425,18 @@
         <f t="shared" si="2"/>
         <v>31646</v>
       </c>
-      <c r="Q12" s="262">
+      <c r="Q12" s="222">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R12" s="38" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+      <c r="S12" s="147">
+        <v>44495</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="23"/>
       <c r="B13" s="24">
         <v>44496</v>
@@ -3351,7 +3445,7 @@
         <v>2890</v>
       </c>
       <c r="D13" s="42" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E13" s="27">
         <v>44496</v>
@@ -3383,15 +3477,18 @@
         <f t="shared" si="2"/>
         <v>28816.35</v>
       </c>
-      <c r="Q13" s="259">
+      <c r="Q13" s="219">
         <f t="shared" si="1"/>
         <v>1016.3499999999985</v>
       </c>
-      <c r="R13" s="257" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R13" s="217" t="s">
+        <v>43</v>
+      </c>
+      <c r="S13" s="147">
+        <v>44496</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="23"/>
       <c r="B14" s="24">
         <v>44497</v>
@@ -3400,7 +3497,7 @@
         <v>4910</v>
       </c>
       <c r="D14" s="40" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E14" s="27">
         <v>44497</v>
@@ -3429,15 +3526,18 @@
         <f t="shared" ref="P14" si="3">N14+M14+L14+I14+C14</f>
         <v>32621</v>
       </c>
-      <c r="Q14" s="261">
+      <c r="Q14" s="221">
         <f t="shared" si="1"/>
         <v>177</v>
       </c>
-      <c r="R14" s="257" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R14" s="217" t="s">
+        <v>43</v>
+      </c>
+      <c r="S14" s="147">
+        <v>44497</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="23"/>
       <c r="B15" s="24">
         <v>44498</v>
@@ -3446,7 +3546,7 @@
         <v>9347.5</v>
       </c>
       <c r="D15" s="40" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E15" s="27">
         <v>44498</v>
@@ -3474,15 +3574,18 @@
         <f t="shared" si="0"/>
         <v>28788.5</v>
       </c>
-      <c r="Q15" s="258">
+      <c r="Q15" s="218">
         <f t="shared" si="1"/>
         <v>-2472.5</v>
       </c>
-      <c r="R15" s="256" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R15" s="216" t="s">
+        <v>32</v>
+      </c>
+      <c r="S15" s="147">
+        <v>44498</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="23"/>
       <c r="B16" s="24">
         <v>44499</v>
@@ -3491,7 +3594,7 @@
         <v>1588</v>
       </c>
       <c r="D16" s="35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E16" s="27">
         <v>44499</v>
@@ -3519,12 +3622,15 @@
         <f t="shared" si="0"/>
         <v>49883</v>
       </c>
-      <c r="Q16" s="263">
+      <c r="Q16" s="223">
         <f t="shared" si="1"/>
         <v>1942</v>
       </c>
-      <c r="R16" s="257" t="s">
-        <v>44</v>
+      <c r="R16" s="217" t="s">
+        <v>43</v>
+      </c>
+      <c r="S16" s="147">
+        <v>44499</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -3562,12 +3668,15 @@
         <f t="shared" si="0"/>
         <v>38871.5</v>
       </c>
-      <c r="Q17" s="263">
+      <c r="Q17" s="223">
         <f t="shared" si="1"/>
         <v>378.5</v>
       </c>
-      <c r="R17" s="257" t="s">
-        <v>44</v>
+      <c r="R17" s="217" t="s">
+        <v>43</v>
+      </c>
+      <c r="S17" s="147">
+        <v>44500</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -3579,7 +3688,7 @@
         <v>1225</v>
       </c>
       <c r="D18" s="35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E18" s="27">
         <v>44501</v>
@@ -3598,7 +3707,7 @@
         <v>44501</v>
       </c>
       <c r="K18" s="183" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L18" s="39">
         <v>1440</v>
@@ -3614,12 +3723,15 @@
         <f t="shared" si="0"/>
         <v>39738</v>
       </c>
-      <c r="Q18" s="260">
+      <c r="Q18" s="220">
         <f t="shared" si="1"/>
         <v>-3452</v>
       </c>
-      <c r="R18" s="256" t="s">
-        <v>33</v>
+      <c r="R18" s="216" t="s">
+        <v>32</v>
+      </c>
+      <c r="S18" s="147">
+        <v>44501</v>
       </c>
     </row>
     <row r="19" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -3632,7 +3744,7 @@
         <v>23164</v>
       </c>
       <c r="D19" s="35" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E19" s="27">
         <v>44502</v>
@@ -3660,12 +3772,15 @@
         <f t="shared" si="0"/>
         <v>37356.5</v>
       </c>
-      <c r="Q19" s="260">
+      <c r="Q19" s="220">
         <f t="shared" si="1"/>
         <v>-822.5</v>
       </c>
-      <c r="R19" s="256" t="s">
-        <v>33</v>
+      <c r="R19" s="216" t="s">
+        <v>32</v>
+      </c>
+      <c r="S19" s="147">
+        <v>44502</v>
       </c>
     </row>
     <row r="20" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -3678,7 +3793,7 @@
         <v>33449.9</v>
       </c>
       <c r="D20" s="35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E20" s="27">
         <v>44503</v>
@@ -3706,11 +3821,14 @@
         <f t="shared" si="0"/>
         <v>39315.9</v>
       </c>
-      <c r="Q20" s="262">
+      <c r="Q20" s="222">
         <f t="shared" si="1"/>
         <v>0.90000000000145519</v>
       </c>
       <c r="R20" s="38"/>
+      <c r="S20" s="147">
+        <v>44503</v>
+      </c>
     </row>
     <row r="21" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="23"/>
@@ -3722,7 +3840,7 @@
         <v>35613</v>
       </c>
       <c r="D21" s="35" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E21" s="27">
         <v>44504</v>
@@ -3750,11 +3868,14 @@
         <f t="shared" si="0"/>
         <v>43752</v>
       </c>
-      <c r="Q21" s="262">
+      <c r="Q21" s="222">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R21" s="38"/>
+      <c r="S21" s="147">
+        <v>44504</v>
+      </c>
     </row>
     <row r="22" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="23"/>
@@ -3765,7 +3886,7 @@
         <v>1777</v>
       </c>
       <c r="D22" s="35" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E22" s="27">
         <v>44505</v>
@@ -3793,12 +3914,15 @@
         <f t="shared" si="0"/>
         <v>29504</v>
       </c>
-      <c r="Q22" s="260">
+      <c r="Q22" s="220">
         <f t="shared" si="1"/>
         <v>-1457</v>
       </c>
-      <c r="R22" s="256" t="s">
-        <v>33</v>
+      <c r="R22" s="216" t="s">
+        <v>32</v>
+      </c>
+      <c r="S22" s="147">
+        <v>44505</v>
       </c>
     </row>
     <row r="23" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -3811,7 +3935,7 @@
         <v>2606</v>
       </c>
       <c r="D23" s="35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E23" s="27">
         <v>44506</v>
@@ -3830,7 +3954,7 @@
         <v>44506</v>
       </c>
       <c r="K23" s="185" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L23" s="45">
         <v>23657.14</v>
@@ -3845,12 +3969,15 @@
         <f t="shared" si="0"/>
         <v>50727.14</v>
       </c>
-      <c r="Q23" s="260">
+      <c r="Q23" s="220">
         <f t="shared" si="1"/>
         <v>-18819.86</v>
       </c>
-      <c r="R23" s="256" t="s">
-        <v>33</v>
+      <c r="R23" s="216" t="s">
+        <v>32</v>
+      </c>
+      <c r="S23" s="147">
+        <v>44506</v>
       </c>
     </row>
     <row r="24" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -3888,12 +4015,15 @@
         <f t="shared" si="0"/>
         <v>9868.5</v>
       </c>
-      <c r="Q24" s="260">
+      <c r="Q24" s="220">
         <f t="shared" si="1"/>
         <v>-24335.5</v>
       </c>
-      <c r="R24" s="256" t="s">
-        <v>33</v>
+      <c r="R24" s="216" t="s">
+        <v>32</v>
+      </c>
+      <c r="S24" s="147">
+        <v>44507</v>
       </c>
     </row>
     <row r="25" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -3915,11 +4045,11 @@
       <c r="N25" s="33">
         <v>0</v>
       </c>
-      <c r="P25" s="69">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q25" s="9">
+      <c r="P25" s="232">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q25" s="233">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3928,7 +4058,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:19" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="23"/>
       <c r="B26" s="24"/>
       <c r="C26" s="25"/>
@@ -3947,7 +4077,7 @@
       <c r="N26" s="33">
         <v>0</v>
       </c>
-      <c r="P26" s="69">
+      <c r="P26" s="231">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3957,7 +4087,7 @@
       </c>
       <c r="R26" s="31"/>
     </row>
-    <row r="27" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:19" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="23"/>
       <c r="B27" s="24"/>
       <c r="C27" s="25"/>
@@ -4257,7 +4387,7 @@
       </c>
       <c r="R36" s="31"/>
     </row>
-    <row r="37" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:18" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="23"/>
       <c r="B37" s="24"/>
       <c r="C37" s="25">
@@ -4286,7 +4416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:18" ht="18" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="23"/>
       <c r="B38" s="24"/>
       <c r="C38" s="25">
@@ -4328,11 +4458,11 @@
       <c r="J39" s="60"/>
       <c r="K39" s="190"/>
       <c r="L39" s="61"/>
-      <c r="M39" s="223">
+      <c r="M39" s="253">
         <f>SUM(M5:M38)</f>
         <v>247061</v>
       </c>
-      <c r="N39" s="225">
+      <c r="N39" s="255">
         <f>SUM(N5:N38)</f>
         <v>172863</v>
       </c>
@@ -4340,7 +4470,7 @@
         <f>SUM(P5:P38)</f>
         <v>626289.39</v>
       </c>
-      <c r="Q39" s="13">
+      <c r="Q39" s="234">
         <f>SUM(Q5:Q38)</f>
         <v>-53663.11</v>
       </c>
@@ -4358,8 +4488,8 @@
       <c r="J40" s="60"/>
       <c r="K40" s="41"/>
       <c r="L40" s="61"/>
-      <c r="M40" s="224"/>
-      <c r="N40" s="226"/>
+      <c r="M40" s="254"/>
+      <c r="N40" s="256"/>
       <c r="P40" s="34"/>
       <c r="Q40" s="9"/>
     </row>
@@ -4574,29 +4704,29 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="227" t="s">
+      <c r="H52" s="257" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="228"/>
+      <c r="I52" s="258"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="229">
+      <c r="K52" s="259">
         <f>I50+L50</f>
         <v>53873.49</v>
       </c>
-      <c r="L52" s="230"/>
-      <c r="M52" s="231">
+      <c r="L52" s="260"/>
+      <c r="M52" s="261">
         <f>N39+M39</f>
         <v>419924</v>
       </c>
-      <c r="N52" s="232"/>
+      <c r="N52" s="262"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="233" t="s">
+      <c r="D53" s="263" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="233"/>
+      <c r="E53" s="263"/>
       <c r="F53" s="101">
         <f>F50-K52-C50</f>
         <v>471038.61</v>
@@ -4607,28 +4737,28 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="233" t="s">
-        <v>102</v>
-      </c>
-      <c r="E54" s="233"/>
+      <c r="D54" s="263" t="s">
+        <v>101</v>
+      </c>
+      <c r="E54" s="263"/>
       <c r="F54" s="96">
-        <v>-409976.4</v>
-      </c>
-      <c r="I54" s="234" t="s">
+        <v>-549976.4</v>
+      </c>
+      <c r="I54" s="264" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="235"/>
-      <c r="K54" s="236">
+      <c r="J54" s="265"/>
+      <c r="K54" s="266">
         <f>F56+F57+F58</f>
-        <v>115422.59999999992</v>
-      </c>
-      <c r="L54" s="237"/>
+        <v>-24577.400000000023</v>
+      </c>
+      <c r="L54" s="267"/>
       <c r="P54" s="34"/>
       <c r="Q54" s="9"/>
     </row>
     <row r="55" spans="1:17" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D55" s="203" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E55" s="98"/>
       <c r="F55" s="104">
@@ -4648,18 +4778,18 @@
       </c>
       <c r="F56" s="96">
         <f>SUM(F53:F55)</f>
-        <v>-451966.75000000006</v>
+        <v>-591966.75</v>
       </c>
       <c r="H56" s="23"/>
       <c r="I56" s="108" t="s">
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="238">
+      <c r="K56" s="268">
         <f>-C4</f>
         <v>0</v>
       </c>
-      <c r="L56" s="239"/>
+      <c r="L56" s="269"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -4676,22 +4806,22 @@
       <c r="C58" s="112">
         <v>44507</v>
       </c>
-      <c r="D58" s="216" t="s">
+      <c r="D58" s="246" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="217"/>
+      <c r="E58" s="247"/>
       <c r="F58" s="113">
         <v>567389.35</v>
       </c>
-      <c r="I58" s="218" t="s">
-        <v>19</v>
-      </c>
-      <c r="J58" s="219"/>
-      <c r="K58" s="220">
+      <c r="I58" s="248" t="s">
+        <v>103</v>
+      </c>
+      <c r="J58" s="249"/>
+      <c r="K58" s="250">
         <f>K54+K56</f>
-        <v>115422.59999999992</v>
-      </c>
-      <c r="L58" s="220"/>
+        <v>-24577.400000000023</v>
+      </c>
+      <c r="L58" s="250"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -4870,8 +5000,8 @@
   </sheetPr>
   <dimension ref="A1:N134"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="Q54" sqref="Q54"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="J98" sqref="J98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4893,62 +5023,62 @@
   <sheetData>
     <row r="1" spans="1:14" ht="36.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="166" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B1" s="167"/>
       <c r="C1" s="168"/>
       <c r="D1" s="167"/>
       <c r="E1" s="168"/>
       <c r="F1" s="169" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I1" s="200" t="s">
-        <v>98</v>
-      </c>
-      <c r="J1" s="247"/>
+        <v>97</v>
+      </c>
+      <c r="J1" s="207"/>
       <c r="K1" s="202"/>
       <c r="L1" s="201"/>
       <c r="M1" s="202"/>
       <c r="N1" s="169" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="131" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="131" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="131" t="s">
+      <c r="C2" s="132" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="132" t="s">
+      <c r="D2" s="131" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="131" t="s">
+      <c r="E2" s="132" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="132" t="s">
-        <v>24</v>
-      </c>
       <c r="F2" s="133" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="131" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="206" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="132" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="131" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="131" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="246" t="s">
+      <c r="M2" s="132" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" s="133" t="s">
         <v>21</v>
-      </c>
-      <c r="K2" s="132" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" s="131" t="s">
-        <v>23</v>
-      </c>
-      <c r="M2" s="132" t="s">
-        <v>24</v>
-      </c>
-      <c r="N2" s="133" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -4956,7 +5086,7 @@
         <v>44487</v>
       </c>
       <c r="B3" s="135" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" s="69">
         <v>225686.58</v>
@@ -4967,13 +5097,13 @@
         <f>C3-E3</f>
         <v>225686.58</v>
       </c>
-      <c r="I3" s="245">
+      <c r="I3" s="205">
         <v>44483</v>
       </c>
-      <c r="J3" s="249">
+      <c r="J3" s="209">
         <v>2554</v>
       </c>
-      <c r="K3" s="250">
+      <c r="K3" s="210">
         <v>19269</v>
       </c>
       <c r="L3" s="136"/>
@@ -4988,7 +5118,7 @@
         <v>44488</v>
       </c>
       <c r="B4" s="135" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C4" s="69">
         <v>53647.199999999997</v>
@@ -5000,13 +5130,13 @@
         <v>279333.77999999997</v>
       </c>
       <c r="G4" s="138"/>
-      <c r="I4" s="245">
+      <c r="I4" s="205">
         <v>44487</v>
       </c>
-      <c r="J4" s="249">
+      <c r="J4" s="209">
         <v>2579</v>
       </c>
-      <c r="K4" s="250">
+      <c r="K4" s="210">
         <v>25542</v>
       </c>
       <c r="L4" s="136"/>
@@ -5021,7 +5151,7 @@
         <v>44488</v>
       </c>
       <c r="B5" s="135" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C5" s="69">
         <v>117061.64</v>
@@ -5032,13 +5162,13 @@
         <f t="shared" ref="F5:F68" si="0">F4+C5-E5</f>
         <v>396395.42</v>
       </c>
-      <c r="I5" s="245">
+      <c r="I5" s="205">
         <v>44487</v>
       </c>
-      <c r="J5" s="249">
+      <c r="J5" s="209">
         <v>2581</v>
       </c>
-      <c r="K5" s="250">
+      <c r="K5" s="210">
         <v>10208</v>
       </c>
       <c r="L5" s="136"/>
@@ -5053,7 +5183,7 @@
         <v>44488</v>
       </c>
       <c r="B6" s="135" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6" s="69">
         <v>1300</v>
@@ -5064,13 +5194,13 @@
         <f t="shared" si="0"/>
         <v>397695.42</v>
       </c>
-      <c r="I6" s="245">
+      <c r="I6" s="205">
         <v>44487</v>
       </c>
-      <c r="J6" s="249">
+      <c r="J6" s="209">
         <v>2582</v>
       </c>
-      <c r="K6" s="250">
+      <c r="K6" s="210">
         <v>14172</v>
       </c>
       <c r="L6" s="136"/>
@@ -5085,7 +5215,7 @@
         <v>44488</v>
       </c>
       <c r="B7" s="135" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C7" s="69">
         <v>1741.6</v>
@@ -5096,13 +5226,13 @@
         <f t="shared" si="0"/>
         <v>399437.01999999996</v>
       </c>
-      <c r="I7" s="245">
+      <c r="I7" s="205">
         <v>44487</v>
       </c>
-      <c r="J7" s="249">
+      <c r="J7" s="209">
         <v>2583</v>
       </c>
-      <c r="K7" s="250">
+      <c r="K7" s="210">
         <v>1616</v>
       </c>
       <c r="L7" s="136"/>
@@ -5117,7 +5247,7 @@
         <v>44489</v>
       </c>
       <c r="B8" s="135" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C8" s="69">
         <v>15000</v>
@@ -5128,13 +5258,13 @@
         <f t="shared" si="0"/>
         <v>414437.01999999996</v>
       </c>
-      <c r="I8" s="245">
+      <c r="I8" s="205">
         <v>44488</v>
       </c>
-      <c r="J8" s="249">
+      <c r="J8" s="209">
         <v>2591</v>
       </c>
-      <c r="K8" s="250">
+      <c r="K8" s="210">
         <v>15642</v>
       </c>
       <c r="L8" s="136"/>
@@ -5149,7 +5279,7 @@
         <v>44489</v>
       </c>
       <c r="B9" s="135" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C9" s="69">
         <v>23362.9</v>
@@ -5160,13 +5290,13 @@
         <f t="shared" si="0"/>
         <v>437799.92</v>
       </c>
-      <c r="I9" s="245">
+      <c r="I9" s="205">
         <v>44488</v>
       </c>
-      <c r="J9" s="249">
+      <c r="J9" s="209">
         <v>2592</v>
       </c>
-      <c r="K9" s="250">
+      <c r="K9" s="210">
         <v>13192</v>
       </c>
       <c r="L9" s="136"/>
@@ -5181,7 +5311,7 @@
         <v>44489</v>
       </c>
       <c r="B10" s="135" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C10" s="69">
         <v>199330</v>
@@ -5193,13 +5323,13 @@
         <v>637129.91999999993</v>
       </c>
       <c r="G10" s="138"/>
-      <c r="I10" s="245">
+      <c r="I10" s="205">
         <v>44488</v>
       </c>
-      <c r="J10" s="249">
+      <c r="J10" s="209">
         <v>2593</v>
       </c>
-      <c r="K10" s="250">
+      <c r="K10" s="210">
         <v>21530</v>
       </c>
       <c r="L10" s="136"/>
@@ -5214,7 +5344,7 @@
         <v>44489</v>
       </c>
       <c r="B11" s="139" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C11" s="69">
         <v>198868.1</v>
@@ -5225,13 +5355,13 @@
         <f t="shared" si="0"/>
         <v>835998.0199999999</v>
       </c>
-      <c r="I11" s="245">
+      <c r="I11" s="205">
         <v>44488</v>
       </c>
-      <c r="J11" s="249">
+      <c r="J11" s="209">
         <v>2594</v>
       </c>
-      <c r="K11" s="250">
+      <c r="K11" s="210">
         <v>10768</v>
       </c>
       <c r="L11" s="140"/>
@@ -5245,8 +5375,8 @@
       <c r="A12" s="140">
         <v>44489</v>
       </c>
-      <c r="B12" s="139" t="s">
-        <v>69</v>
+      <c r="B12" s="224" t="s">
+        <v>68</v>
       </c>
       <c r="C12" s="69">
         <v>191153.5</v>
@@ -5257,13 +5387,13 @@
         <f t="shared" si="0"/>
         <v>1027151.5199999999</v>
       </c>
-      <c r="I12" s="245">
+      <c r="I12" s="205">
         <v>44488</v>
       </c>
-      <c r="J12" s="249">
+      <c r="J12" s="209">
         <v>2595</v>
       </c>
-      <c r="K12" s="250">
+      <c r="K12" s="210">
         <v>90060</v>
       </c>
       <c r="L12" s="140"/>
@@ -5278,7 +5408,7 @@
         <v>44498</v>
       </c>
       <c r="B13" s="198" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C13" s="199">
         <v>-1027151.52</v>
@@ -5289,13 +5419,13 @@
         <f t="shared" si="0"/>
         <v>-1.1641532182693481E-10</v>
       </c>
-      <c r="I13" s="245">
+      <c r="I13" s="205">
         <v>44488</v>
       </c>
-      <c r="J13" s="249">
+      <c r="J13" s="209">
         <v>2596</v>
       </c>
-      <c r="K13" s="250">
+      <c r="K13" s="210">
         <v>18321</v>
       </c>
       <c r="L13" s="140"/>
@@ -5309,8 +5439,8 @@
       <c r="A14" s="140">
         <v>44498</v>
       </c>
-      <c r="B14" s="139" t="s">
-        <v>69</v>
+      <c r="B14" s="224" t="s">
+        <v>68</v>
       </c>
       <c r="C14" s="69">
         <v>6239</v>
@@ -5321,13 +5451,13 @@
         <f t="shared" si="0"/>
         <v>6238.9999999998836</v>
       </c>
-      <c r="I14" s="245">
+      <c r="I14" s="205">
         <v>44488</v>
       </c>
-      <c r="J14" s="249">
+      <c r="J14" s="209">
         <v>2597</v>
       </c>
-      <c r="K14" s="250">
+      <c r="K14" s="210">
         <v>20989</v>
       </c>
       <c r="L14" s="140"/>
@@ -5342,7 +5472,7 @@
         <v>44489</v>
       </c>
       <c r="B15" s="139" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C15" s="69">
         <v>2200</v>
@@ -5353,13 +5483,13 @@
         <f t="shared" si="0"/>
         <v>8438.9999999998836</v>
       </c>
-      <c r="I15" s="245">
+      <c r="I15" s="205">
         <v>44488</v>
       </c>
-      <c r="J15" s="249">
+      <c r="J15" s="209">
         <v>2598</v>
       </c>
-      <c r="K15" s="250">
+      <c r="K15" s="210">
         <v>25399</v>
       </c>
       <c r="L15" s="140"/>
@@ -5374,7 +5504,7 @@
         <v>44489</v>
       </c>
       <c r="B16" s="139" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C16" s="69">
         <v>283491.90000000002</v>
@@ -5389,13 +5519,13 @@
         <f t="shared" si="0"/>
         <v>146930.89999999991</v>
       </c>
-      <c r="I16" s="245">
+      <c r="I16" s="205">
         <v>44489</v>
       </c>
-      <c r="J16" s="249">
+      <c r="J16" s="209">
         <v>2600</v>
       </c>
-      <c r="K16" s="250">
+      <c r="K16" s="210">
         <v>6297</v>
       </c>
       <c r="L16" s="140"/>
@@ -5410,7 +5540,7 @@
         <v>44490</v>
       </c>
       <c r="B17" s="139" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C17" s="69">
         <v>19643.5</v>
@@ -5421,13 +5551,13 @@
         <f t="shared" si="0"/>
         <v>166574.39999999991</v>
       </c>
-      <c r="I17" s="245">
+      <c r="I17" s="205">
         <v>44489</v>
       </c>
-      <c r="J17" s="249">
+      <c r="J17" s="209">
         <v>2601</v>
       </c>
-      <c r="K17" s="250">
+      <c r="K17" s="210">
         <v>12350</v>
       </c>
       <c r="L17" s="140"/>
@@ -5442,7 +5572,7 @@
         <v>44490</v>
       </c>
       <c r="B18" s="139" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C18" s="69">
         <v>3737</v>
@@ -5453,13 +5583,13 @@
         <f t="shared" si="0"/>
         <v>170311.39999999991</v>
       </c>
-      <c r="I18" s="245">
+      <c r="I18" s="205">
         <v>44489</v>
       </c>
-      <c r="J18" s="249">
+      <c r="J18" s="209">
         <v>2602</v>
       </c>
-      <c r="K18" s="250">
+      <c r="K18" s="210">
         <v>5444</v>
       </c>
       <c r="L18" s="140"/>
@@ -5474,7 +5604,7 @@
         <v>44491</v>
       </c>
       <c r="B19" s="139" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C19" s="69">
         <v>1072.5</v>
@@ -5485,13 +5615,13 @@
         <f t="shared" si="0"/>
         <v>171383.89999999991</v>
       </c>
-      <c r="I19" s="245">
+      <c r="I19" s="205">
         <v>44489</v>
       </c>
-      <c r="J19" s="249">
+      <c r="J19" s="209">
         <v>2603</v>
       </c>
-      <c r="K19" s="250">
+      <c r="K19" s="210">
         <v>1717</v>
       </c>
       <c r="L19" s="140"/>
@@ -5506,7 +5636,7 @@
         <v>44492</v>
       </c>
       <c r="B20" s="139" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C20" s="69">
         <v>19152.8</v>
@@ -5517,13 +5647,13 @@
         <f t="shared" si="0"/>
         <v>190536.6999999999</v>
       </c>
-      <c r="I20" s="245">
+      <c r="I20" s="205">
         <v>44489</v>
       </c>
-      <c r="J20" s="249">
+      <c r="J20" s="209">
         <v>2608</v>
       </c>
-      <c r="K20" s="250">
+      <c r="K20" s="210">
         <v>16136</v>
       </c>
       <c r="L20" s="140"/>
@@ -5538,7 +5668,7 @@
         <v>44492</v>
       </c>
       <c r="B21" s="139" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C21" s="69">
         <v>2509</v>
@@ -5549,13 +5679,13 @@
         <f t="shared" si="0"/>
         <v>193045.6999999999</v>
       </c>
-      <c r="I21" s="245">
+      <c r="I21" s="205">
         <v>44489</v>
       </c>
-      <c r="J21" s="249">
+      <c r="J21" s="209">
         <v>2609</v>
       </c>
-      <c r="K21" s="250">
+      <c r="K21" s="210">
         <v>9256</v>
       </c>
       <c r="L21" s="140"/>
@@ -5570,7 +5700,7 @@
         <v>44494</v>
       </c>
       <c r="B22" s="139" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C22" s="69">
         <v>1228.5</v>
@@ -5582,13 +5712,13 @@
         <v>194274.1999999999</v>
       </c>
       <c r="G22" s="138"/>
-      <c r="I22" s="245">
+      <c r="I22" s="205">
         <v>44490</v>
       </c>
-      <c r="J22" s="249">
+      <c r="J22" s="209">
         <v>2611</v>
       </c>
-      <c r="K22" s="250">
+      <c r="K22" s="210">
         <v>5500</v>
       </c>
       <c r="L22" s="140"/>
@@ -5603,7 +5733,7 @@
         <v>44495</v>
       </c>
       <c r="B23" s="139" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C23" s="69">
         <v>46234</v>
@@ -5614,13 +5744,13 @@
         <f t="shared" si="0"/>
         <v>240508.1999999999</v>
       </c>
-      <c r="I23" s="245">
+      <c r="I23" s="205">
         <v>44490</v>
       </c>
-      <c r="J23" s="249">
+      <c r="J23" s="209">
         <v>2615</v>
       </c>
-      <c r="K23" s="250">
+      <c r="K23" s="210">
         <v>1331</v>
       </c>
       <c r="L23" s="140"/>
@@ -5635,7 +5765,7 @@
         <v>44495</v>
       </c>
       <c r="B24" s="139" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C24" s="69">
         <v>6250</v>
@@ -5646,13 +5776,13 @@
         <f t="shared" si="0"/>
         <v>246758.1999999999</v>
       </c>
-      <c r="I24" s="245">
+      <c r="I24" s="205">
         <v>44490</v>
       </c>
-      <c r="J24" s="249">
+      <c r="J24" s="209">
         <v>2619</v>
       </c>
-      <c r="K24" s="250">
+      <c r="K24" s="210">
         <v>420</v>
       </c>
       <c r="L24" s="140"/>
@@ -5667,7 +5797,7 @@
         <v>44496</v>
       </c>
       <c r="B25" s="139" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C25" s="69">
         <v>2092.1999999999998</v>
@@ -5678,13 +5808,13 @@
         <f t="shared" si="0"/>
         <v>248850.39999999991</v>
       </c>
-      <c r="I25" s="245">
+      <c r="I25" s="205">
         <v>44490</v>
       </c>
-      <c r="J25" s="249">
+      <c r="J25" s="209">
         <v>2620</v>
       </c>
-      <c r="K25" s="250">
+      <c r="K25" s="210">
         <v>770</v>
       </c>
       <c r="L25" s="140"/>
@@ -5699,7 +5829,7 @@
         <v>44496</v>
       </c>
       <c r="B26" s="139" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C26" s="69">
         <v>2756</v>
@@ -5710,13 +5840,13 @@
         <f t="shared" si="0"/>
         <v>251606.39999999991</v>
       </c>
-      <c r="I26" s="245">
+      <c r="I26" s="205">
         <v>44491</v>
       </c>
-      <c r="J26" s="249">
+      <c r="J26" s="209">
         <v>2622</v>
       </c>
-      <c r="K26" s="250">
+      <c r="K26" s="210">
         <v>2257</v>
       </c>
       <c r="L26" s="140"/>
@@ -5731,7 +5861,7 @@
         <v>44496</v>
       </c>
       <c r="B27" s="139" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C27" s="69">
         <v>9313.6</v>
@@ -5742,13 +5872,13 @@
         <f t="shared" si="0"/>
         <v>260919.99999999991</v>
       </c>
-      <c r="I27" s="245">
+      <c r="I27" s="205">
         <v>44491</v>
       </c>
-      <c r="J27" s="249">
+      <c r="J27" s="209">
         <v>2623</v>
       </c>
-      <c r="K27" s="250">
+      <c r="K27" s="210">
         <v>60</v>
       </c>
       <c r="L27" s="140"/>
@@ -5763,7 +5893,7 @@
         <v>44497</v>
       </c>
       <c r="B28" s="139" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C28" s="69">
         <v>10048.5</v>
@@ -5774,13 +5904,13 @@
         <f t="shared" si="0"/>
         <v>270968.49999999988</v>
       </c>
-      <c r="I28" s="245">
+      <c r="I28" s="205">
         <v>44491</v>
       </c>
-      <c r="J28" s="249">
+      <c r="J28" s="209">
         <v>2628</v>
       </c>
-      <c r="K28" s="250">
+      <c r="K28" s="210">
         <v>39533</v>
       </c>
       <c r="L28" s="140"/>
@@ -5795,7 +5925,7 @@
         <v>44497</v>
       </c>
       <c r="B29" s="139" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C29" s="69">
         <v>3233</v>
@@ -5806,13 +5936,13 @@
         <f t="shared" si="0"/>
         <v>274201.49999999988</v>
       </c>
-      <c r="I29" s="245">
+      <c r="I29" s="205">
         <v>44492</v>
       </c>
-      <c r="J29" s="249">
+      <c r="J29" s="209">
         <v>2633</v>
       </c>
-      <c r="K29" s="250">
+      <c r="K29" s="210">
         <v>3727</v>
       </c>
       <c r="L29" s="140"/>
@@ -5827,7 +5957,7 @@
         <v>44498</v>
       </c>
       <c r="B30" s="139" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C30" s="69">
         <v>18440.3</v>
@@ -5839,13 +5969,13 @@
         <v>292641.79999999987</v>
       </c>
       <c r="G30" s="138"/>
-      <c r="I30" s="245">
+      <c r="I30" s="205">
         <v>44493</v>
       </c>
-      <c r="J30" s="251">
+      <c r="J30" s="211">
         <v>2638</v>
       </c>
-      <c r="K30" s="252">
+      <c r="K30" s="212">
         <v>3861</v>
       </c>
       <c r="L30" s="140"/>
@@ -5860,7 +5990,7 @@
         <v>44498</v>
       </c>
       <c r="B31" s="139" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C31" s="69">
         <v>5634.12</v>
@@ -5871,13 +6001,13 @@
         <f t="shared" si="0"/>
         <v>298275.91999999987</v>
       </c>
-      <c r="I31" s="245">
+      <c r="I31" s="205">
         <v>44493</v>
       </c>
-      <c r="J31" s="249">
+      <c r="J31" s="209">
         <v>2641</v>
       </c>
-      <c r="K31" s="250">
+      <c r="K31" s="210">
         <v>24825</v>
       </c>
       <c r="L31" s="140"/>
@@ -5892,7 +6022,7 @@
         <v>44499</v>
       </c>
       <c r="B32" s="139" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C32" s="69">
         <v>42852</v>
@@ -5903,13 +6033,13 @@
         <f t="shared" si="0"/>
         <v>341127.91999999987</v>
       </c>
-      <c r="I32" s="245">
+      <c r="I32" s="205">
         <v>44493</v>
       </c>
-      <c r="J32" s="249">
+      <c r="J32" s="209">
         <v>2642</v>
       </c>
-      <c r="K32" s="250">
+      <c r="K32" s="210">
         <v>614</v>
       </c>
       <c r="L32" s="140"/>
@@ -5924,7 +6054,7 @@
         <v>44501</v>
       </c>
       <c r="B33" s="139" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C33" s="69">
         <v>7757.6</v>
@@ -5935,13 +6065,13 @@
         <f t="shared" si="0"/>
         <v>348885.51999999984</v>
       </c>
-      <c r="I33" s="245">
+      <c r="I33" s="205">
         <v>44494</v>
       </c>
-      <c r="J33" s="249">
+      <c r="J33" s="209">
         <v>2644</v>
       </c>
-      <c r="K33" s="250">
+      <c r="K33" s="210">
         <v>2901</v>
       </c>
       <c r="L33" s="140"/>
@@ -5956,7 +6086,7 @@
         <v>44502</v>
       </c>
       <c r="B34" s="139" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C34" s="69">
         <v>6498</v>
@@ -5967,13 +6097,13 @@
         <f t="shared" si="0"/>
         <v>355383.51999999984</v>
       </c>
-      <c r="I34" s="245">
+      <c r="I34" s="205">
         <v>44495</v>
       </c>
-      <c r="J34" s="249">
+      <c r="J34" s="209">
         <v>2648</v>
       </c>
-      <c r="K34" s="250">
+      <c r="K34" s="210">
         <v>2623</v>
       </c>
       <c r="L34" s="140"/>
@@ -5988,7 +6118,7 @@
         <v>44504</v>
       </c>
       <c r="B35" s="139" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C35" s="69">
         <v>5926.3</v>
@@ -5999,13 +6129,13 @@
         <f t="shared" si="0"/>
         <v>361309.81999999983</v>
       </c>
-      <c r="I35" s="245">
+      <c r="I35" s="205">
         <v>44495</v>
       </c>
-      <c r="J35" s="249">
+      <c r="J35" s="209">
         <v>2653</v>
       </c>
-      <c r="K35" s="250">
+      <c r="K35" s="210">
         <v>740</v>
       </c>
       <c r="L35" s="140"/>
@@ -6020,7 +6150,7 @@
         <v>44505</v>
       </c>
       <c r="B36" s="139" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C36" s="69">
         <v>19420.8</v>
@@ -6031,13 +6161,13 @@
         <f t="shared" si="0"/>
         <v>380730.61999999982</v>
       </c>
-      <c r="I36" s="245">
+      <c r="I36" s="205">
         <v>44495</v>
       </c>
-      <c r="J36" s="251">
+      <c r="J36" s="211">
         <v>2655</v>
       </c>
-      <c r="K36" s="252">
+      <c r="K36" s="212">
         <v>1189</v>
       </c>
       <c r="L36" s="140"/>
@@ -6052,7 +6182,7 @@
         <v>44505</v>
       </c>
       <c r="B37" s="139" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C37" s="69">
         <v>10233.200000000001</v>
@@ -6063,13 +6193,13 @@
         <f t="shared" si="0"/>
         <v>390963.81999999983</v>
       </c>
-      <c r="I37" s="245">
+      <c r="I37" s="205">
         <v>44496</v>
       </c>
-      <c r="J37" s="249">
+      <c r="J37" s="209">
         <v>2659</v>
       </c>
-      <c r="K37" s="250">
+      <c r="K37" s="210">
         <v>6711</v>
       </c>
       <c r="L37" s="140"/>
@@ -6084,7 +6214,7 @@
         <v>44506</v>
       </c>
       <c r="B38" s="139" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C38" s="69">
         <v>15301.7</v>
@@ -6095,13 +6225,13 @@
         <f t="shared" si="0"/>
         <v>406265.51999999984</v>
       </c>
-      <c r="I38" s="245">
+      <c r="I38" s="205">
         <v>44497</v>
       </c>
-      <c r="J38" s="249">
+      <c r="J38" s="209">
         <v>2666</v>
       </c>
-      <c r="K38" s="250">
+      <c r="K38" s="210">
         <v>71111</v>
       </c>
       <c r="L38" s="140"/>
@@ -6116,7 +6246,7 @@
         <v>44506</v>
       </c>
       <c r="B39" s="139" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C39" s="69">
         <v>3101.84</v>
@@ -6127,13 +6257,13 @@
         <f t="shared" si="0"/>
         <v>409367.35999999987</v>
       </c>
-      <c r="I39" s="245">
+      <c r="I39" s="205">
         <v>44497</v>
       </c>
-      <c r="J39" s="249">
+      <c r="J39" s="209">
         <v>2668</v>
       </c>
-      <c r="K39" s="250">
+      <c r="K39" s="210">
         <v>13525</v>
       </c>
       <c r="L39" s="140"/>
@@ -6148,7 +6278,7 @@
         <v>44506</v>
       </c>
       <c r="B40" s="139" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C40" s="69">
         <v>81.599999999999994</v>
@@ -6159,13 +6289,13 @@
         <f t="shared" si="0"/>
         <v>409448.95999999985</v>
       </c>
-      <c r="I40" s="245">
+      <c r="I40" s="205">
         <v>44497</v>
       </c>
-      <c r="J40" s="249">
+      <c r="J40" s="209">
         <v>2669</v>
       </c>
-      <c r="K40" s="250">
+      <c r="K40" s="210">
         <v>7227</v>
       </c>
       <c r="L40" s="140"/>
@@ -6179,8 +6309,8 @@
       <c r="A41" s="140">
         <v>44507</v>
       </c>
-      <c r="B41" s="240" t="s">
-        <v>99</v>
+      <c r="B41" s="270" t="s">
+        <v>98</v>
       </c>
       <c r="C41" s="204">
         <v>-4472.5600000000004</v>
@@ -6191,13 +6321,13 @@
         <f t="shared" si="0"/>
         <v>404976.39999999985</v>
       </c>
-      <c r="I41" s="245">
+      <c r="I41" s="205">
         <v>44497</v>
       </c>
-      <c r="J41" s="249">
+      <c r="J41" s="209">
         <v>2672</v>
       </c>
-      <c r="K41" s="250">
+      <c r="K41" s="210">
         <v>2618</v>
       </c>
       <c r="L41" s="140"/>
@@ -6209,9 +6339,9 @@
     </row>
     <row r="42" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="140" t="s">
-        <v>100</v>
-      </c>
-      <c r="B42" s="241"/>
+        <v>99</v>
+      </c>
+      <c r="B42" s="271"/>
       <c r="C42" s="143">
         <v>0</v>
       </c>
@@ -6221,13 +6351,13 @@
         <f t="shared" si="0"/>
         <v>404976.39999999985</v>
       </c>
-      <c r="I42" s="245">
+      <c r="I42" s="205">
         <v>44498</v>
       </c>
-      <c r="J42" s="249">
+      <c r="J42" s="209">
         <v>2675</v>
       </c>
-      <c r="K42" s="250">
+      <c r="K42" s="210">
         <v>8371</v>
       </c>
       <c r="L42" s="140"/>
@@ -6247,13 +6377,13 @@
         <f t="shared" si="0"/>
         <v>404976.39999999985</v>
       </c>
-      <c r="I43" s="245">
+      <c r="I43" s="205">
         <v>44498</v>
       </c>
-      <c r="J43" s="249">
+      <c r="J43" s="209">
         <v>2676</v>
       </c>
-      <c r="K43" s="250">
+      <c r="K43" s="210">
         <v>753</v>
       </c>
       <c r="L43" s="140"/>
@@ -6273,13 +6403,13 @@
         <f t="shared" si="0"/>
         <v>404976.39999999985</v>
       </c>
-      <c r="I44" s="245">
+      <c r="I44" s="205">
         <v>44498</v>
       </c>
-      <c r="J44" s="253" t="s">
-        <v>103</v>
-      </c>
-      <c r="K44" s="254">
+      <c r="J44" s="213" t="s">
+        <v>102</v>
+      </c>
+      <c r="K44" s="214">
         <v>-51341.58</v>
       </c>
       <c r="L44" s="140"/>
@@ -6299,13 +6429,13 @@
         <f t="shared" si="0"/>
         <v>404976.39999999985</v>
       </c>
-      <c r="I45" s="245">
+      <c r="I45" s="205">
         <v>44499</v>
       </c>
-      <c r="J45" s="249">
+      <c r="J45" s="209">
         <v>2684</v>
       </c>
-      <c r="K45" s="250">
+      <c r="K45" s="210">
         <v>5240</v>
       </c>
       <c r="L45" s="140"/>
@@ -6325,13 +6455,13 @@
         <f t="shared" si="0"/>
         <v>404976.39999999985</v>
       </c>
-      <c r="I46" s="245">
+      <c r="I46" s="205">
         <v>44501</v>
       </c>
-      <c r="J46" s="249">
+      <c r="J46" s="209">
         <v>2691</v>
       </c>
-      <c r="K46" s="250">
+      <c r="K46" s="210">
         <v>15576</v>
       </c>
       <c r="L46" s="140"/>
@@ -6351,13 +6481,13 @@
         <f t="shared" si="0"/>
         <v>404976.39999999985</v>
       </c>
-      <c r="I47" s="245">
+      <c r="I47" s="205">
         <v>44501</v>
       </c>
-      <c r="J47" s="249">
+      <c r="J47" s="209">
         <v>2692</v>
       </c>
-      <c r="K47" s="250">
+      <c r="K47" s="210">
         <v>739</v>
       </c>
       <c r="L47" s="140"/>
@@ -6377,13 +6507,13 @@
         <f t="shared" si="0"/>
         <v>404976.39999999985</v>
       </c>
-      <c r="I48" s="245">
+      <c r="I48" s="205">
         <v>44501</v>
       </c>
-      <c r="J48" s="249">
+      <c r="J48" s="209">
         <v>2693</v>
       </c>
-      <c r="K48" s="250">
+      <c r="K48" s="210">
         <v>623</v>
       </c>
       <c r="L48" s="140"/>
@@ -6403,13 +6533,13 @@
         <f t="shared" si="0"/>
         <v>404976.39999999985</v>
       </c>
-      <c r="I49" s="245">
+      <c r="I49" s="205">
         <v>44502</v>
       </c>
-      <c r="J49" s="249">
+      <c r="J49" s="209">
         <v>2700</v>
       </c>
-      <c r="K49" s="250">
+      <c r="K49" s="210">
         <v>2636</v>
       </c>
       <c r="L49" s="140"/>
@@ -6429,13 +6559,13 @@
         <f t="shared" si="0"/>
         <v>404976.39999999985</v>
       </c>
-      <c r="I50" s="245">
+      <c r="I50" s="205">
         <v>44502</v>
       </c>
-      <c r="J50" s="249">
+      <c r="J50" s="209">
         <v>2702</v>
       </c>
-      <c r="K50" s="250">
+      <c r="K50" s="210">
         <v>120</v>
       </c>
       <c r="L50" s="140"/>
@@ -6455,13 +6585,13 @@
         <f t="shared" si="0"/>
         <v>404976.39999999985</v>
       </c>
-      <c r="I51" s="245">
+      <c r="I51" s="205">
         <v>44503</v>
       </c>
-      <c r="J51" s="249">
+      <c r="J51" s="209">
         <v>2711</v>
       </c>
-      <c r="K51" s="250">
+      <c r="K51" s="210">
         <v>14669</v>
       </c>
       <c r="L51" s="140"/>
@@ -6481,13 +6611,13 @@
         <f t="shared" si="0"/>
         <v>404976.39999999985</v>
       </c>
-      <c r="I52" s="245">
+      <c r="I52" s="205">
         <v>44504</v>
       </c>
-      <c r="J52" s="249">
+      <c r="J52" s="209">
         <v>2712</v>
       </c>
-      <c r="K52" s="250">
+      <c r="K52" s="210">
         <v>2897</v>
       </c>
       <c r="L52" s="140"/>
@@ -6507,13 +6637,13 @@
         <f t="shared" si="0"/>
         <v>404976.39999999985</v>
       </c>
-      <c r="I53" s="245">
+      <c r="I53" s="205">
         <v>44504</v>
       </c>
-      <c r="J53" s="249">
+      <c r="J53" s="209">
         <v>2717</v>
       </c>
-      <c r="K53" s="250">
+      <c r="K53" s="210">
         <v>360</v>
       </c>
       <c r="L53" s="140"/>
@@ -6533,13 +6663,13 @@
         <f t="shared" si="0"/>
         <v>404976.39999999985</v>
       </c>
-      <c r="I54" s="245">
+      <c r="I54" s="205">
         <v>44505</v>
       </c>
-      <c r="J54" s="249">
+      <c r="J54" s="209">
         <v>2722</v>
       </c>
-      <c r="K54" s="250">
+      <c r="K54" s="210">
         <v>4820</v>
       </c>
       <c r="L54" s="140"/>
@@ -6559,13 +6689,13 @@
         <f t="shared" si="0"/>
         <v>404976.39999999985</v>
       </c>
-      <c r="I55" s="245">
+      <c r="I55" s="205">
         <v>44505</v>
       </c>
-      <c r="J55" s="249">
+      <c r="J55" s="209">
         <v>2724</v>
       </c>
-      <c r="K55" s="250">
+      <c r="K55" s="210">
         <v>4925</v>
       </c>
       <c r="L55" s="140"/>
@@ -6585,13 +6715,13 @@
         <f t="shared" si="0"/>
         <v>404976.39999999985</v>
       </c>
-      <c r="I56" s="245">
+      <c r="I56" s="205">
         <v>44506</v>
       </c>
-      <c r="J56" s="249">
+      <c r="J56" s="209">
         <v>2732</v>
       </c>
-      <c r="K56" s="250">
+      <c r="K56" s="210">
         <v>5</v>
       </c>
       <c r="L56" s="140"/>
@@ -6611,13 +6741,13 @@
         <f t="shared" si="0"/>
         <v>404976.39999999985</v>
       </c>
-      <c r="I57" s="245">
+      <c r="I57" s="205">
         <v>44506</v>
       </c>
-      <c r="J57" s="249">
+      <c r="J57" s="209">
         <v>2733</v>
       </c>
-      <c r="K57" s="250">
+      <c r="K57" s="210">
         <v>6665</v>
       </c>
       <c r="L57" s="140"/>
@@ -6637,13 +6767,13 @@
         <f t="shared" si="0"/>
         <v>404976.39999999985</v>
       </c>
-      <c r="I58" s="245">
+      <c r="I58" s="205">
         <v>44507</v>
       </c>
-      <c r="J58" s="249">
+      <c r="J58" s="209">
         <v>2738</v>
       </c>
-      <c r="K58" s="250">
+      <c r="K58" s="210">
         <v>646</v>
       </c>
       <c r="L58" s="140"/>
@@ -6663,13 +6793,13 @@
         <f t="shared" si="0"/>
         <v>404976.39999999985</v>
       </c>
-      <c r="I59" s="245">
+      <c r="I59" s="205">
         <v>44507</v>
       </c>
-      <c r="J59" s="253" t="s">
-        <v>103</v>
-      </c>
-      <c r="K59" s="254">
+      <c r="J59" s="213" t="s">
+        <v>102</v>
+      </c>
+      <c r="K59" s="214">
         <v>-34125.46</v>
       </c>
       <c r="L59" s="140"/>
@@ -6719,7 +6849,7 @@
         <v>513028.9599999999</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="134"/>
       <c r="B62" s="139"/>
       <c r="C62" s="69"/>
@@ -7421,8 +7551,8 @@
     </row>
     <row r="97" spans="1:14" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="149"/>
-      <c r="B97" s="150"/>
-      <c r="C97" s="151">
+      <c r="B97" s="226"/>
+      <c r="C97" s="34">
         <v>0</v>
       </c>
       <c r="D97" s="152"/>
@@ -7444,8 +7574,8 @@
       </c>
     </row>
     <row r="98" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B98" s="98"/>
-      <c r="C98" s="1">
+      <c r="B98" s="227"/>
+      <c r="C98" s="228">
         <f>SUM(C3:C97)</f>
         <v>549976.39999999967</v>
       </c>
@@ -7458,7 +7588,7 @@
         <f>F97</f>
         <v>404976.39999999985</v>
       </c>
-      <c r="K98" s="1">
+      <c r="K98" s="225">
         <f>SUM(K3:K97)</f>
         <v>513028.9599999999</v>
       </c>
@@ -7472,9 +7602,9 @@
         <v>513028.9599999999</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B99" s="98"/>
-      <c r="C99" s="1"/>
+    <row r="99" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B99" s="229"/>
+      <c r="C99" s="230"/>
       <c r="D99" s="97"/>
       <c r="E99" s="3"/>
       <c r="F99" s="1"/>
@@ -7499,7 +7629,7 @@
       <c r="B101" s="23"/>
       <c r="D101" s="23"/>
       <c r="I101"/>
-      <c r="J101" s="248"/>
+      <c r="J101" s="208"/>
       <c r="L101" s="23"/>
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.25">
@@ -7507,7 +7637,7 @@
       <c r="B102" s="23"/>
       <c r="D102" s="23"/>
       <c r="I102"/>
-      <c r="J102" s="248"/>
+      <c r="J102" s="208"/>
       <c r="L102" s="23"/>
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.25">
@@ -7515,7 +7645,7 @@
       <c r="B103" s="23"/>
       <c r="D103" s="23"/>
       <c r="I103"/>
-      <c r="J103" s="248"/>
+      <c r="J103" s="208"/>
       <c r="L103" s="23"/>
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.25">
@@ -7524,7 +7654,7 @@
       <c r="D104" s="23"/>
       <c r="F104"/>
       <c r="I104"/>
-      <c r="J104" s="248"/>
+      <c r="J104" s="208"/>
       <c r="L104" s="23"/>
       <c r="N104"/>
     </row>
@@ -7534,7 +7664,7 @@
       <c r="D105" s="23"/>
       <c r="F105"/>
       <c r="I105"/>
-      <c r="J105" s="248"/>
+      <c r="J105" s="208"/>
       <c r="L105" s="23"/>
       <c r="N105"/>
     </row>
@@ -7544,7 +7674,7 @@
       <c r="D106" s="23"/>
       <c r="F106"/>
       <c r="I106"/>
-      <c r="J106" s="248"/>
+      <c r="J106" s="208"/>
       <c r="L106" s="23"/>
       <c r="N106"/>
     </row>
@@ -7554,7 +7684,7 @@
       <c r="D107" s="23"/>
       <c r="F107"/>
       <c r="I107"/>
-      <c r="J107" s="248"/>
+      <c r="J107" s="208"/>
       <c r="L107" s="23"/>
       <c r="N107"/>
     </row>
@@ -7564,7 +7694,7 @@
       <c r="D108" s="23"/>
       <c r="F108"/>
       <c r="I108"/>
-      <c r="J108" s="248"/>
+      <c r="J108" s="208"/>
       <c r="L108" s="23"/>
       <c r="N108"/>
     </row>
@@ -7574,7 +7704,7 @@
       <c r="D109" s="23"/>
       <c r="F109"/>
       <c r="I109"/>
-      <c r="J109" s="248"/>
+      <c r="J109" s="208"/>
       <c r="L109" s="23"/>
       <c r="N109"/>
     </row>
@@ -7584,7 +7714,7 @@
       <c r="D110" s="23"/>
       <c r="F110"/>
       <c r="I110"/>
-      <c r="J110" s="248"/>
+      <c r="J110" s="208"/>
       <c r="L110" s="23"/>
       <c r="N110"/>
     </row>
@@ -7594,7 +7724,7 @@
       <c r="D111" s="23"/>
       <c r="F111"/>
       <c r="I111"/>
-      <c r="J111" s="248"/>
+      <c r="J111" s="208"/>
       <c r="L111" s="23"/>
       <c r="N111"/>
     </row>
@@ -7604,7 +7734,7 @@
       <c r="D112" s="23"/>
       <c r="F112"/>
       <c r="I112"/>
-      <c r="J112" s="248"/>
+      <c r="J112" s="208"/>
       <c r="L112" s="23"/>
       <c r="N112"/>
     </row>
@@ -7615,7 +7745,7 @@
       <c r="E113"/>
       <c r="F113"/>
       <c r="I113"/>
-      <c r="J113" s="248"/>
+      <c r="J113" s="208"/>
       <c r="L113" s="23"/>
       <c r="M113"/>
       <c r="N113"/>
@@ -7627,7 +7757,7 @@
       <c r="E114"/>
       <c r="F114"/>
       <c r="I114"/>
-      <c r="J114" s="248"/>
+      <c r="J114" s="208"/>
       <c r="L114" s="23"/>
       <c r="M114"/>
       <c r="N114"/>
@@ -7639,7 +7769,7 @@
       <c r="E115"/>
       <c r="F115"/>
       <c r="I115"/>
-      <c r="J115" s="248"/>
+      <c r="J115" s="208"/>
       <c r="L115" s="23"/>
       <c r="M115"/>
       <c r="N115"/>
@@ -7651,7 +7781,7 @@
       <c r="E116"/>
       <c r="F116"/>
       <c r="I116"/>
-      <c r="J116" s="248"/>
+      <c r="J116" s="208"/>
       <c r="L116" s="23"/>
       <c r="M116"/>
       <c r="N116"/>
@@ -7663,7 +7793,7 @@
       <c r="E117"/>
       <c r="F117"/>
       <c r="I117"/>
-      <c r="J117" s="248"/>
+      <c r="J117" s="208"/>
       <c r="L117" s="23"/>
       <c r="M117"/>
       <c r="N117"/>
@@ -7675,7 +7805,7 @@
       <c r="E118"/>
       <c r="F118"/>
       <c r="I118"/>
-      <c r="J118" s="248"/>
+      <c r="J118" s="208"/>
       <c r="L118" s="23"/>
       <c r="M118"/>
       <c r="N118"/>
@@ -7684,7 +7814,7 @@
       <c r="B119" s="23"/>
       <c r="D119" s="23"/>
       <c r="E119"/>
-      <c r="J119" s="248"/>
+      <c r="J119" s="208"/>
       <c r="L119" s="23"/>
       <c r="M119"/>
     </row>
@@ -7692,7 +7822,7 @@
       <c r="B120" s="23"/>
       <c r="D120" s="23"/>
       <c r="E120"/>
-      <c r="J120" s="248"/>
+      <c r="J120" s="208"/>
       <c r="L120" s="23"/>
       <c r="M120"/>
     </row>
@@ -7700,7 +7830,7 @@
       <c r="B121" s="23"/>
       <c r="D121" s="23"/>
       <c r="E121"/>
-      <c r="J121" s="248"/>
+      <c r="J121" s="208"/>
       <c r="L121" s="23"/>
       <c r="M121"/>
     </row>
@@ -7708,7 +7838,7 @@
       <c r="B122" s="23"/>
       <c r="D122" s="23"/>
       <c r="E122"/>
-      <c r="J122" s="248"/>
+      <c r="J122" s="208"/>
       <c r="L122" s="23"/>
       <c r="M122"/>
     </row>
@@ -7716,7 +7846,7 @@
       <c r="B123" s="23"/>
       <c r="D123" s="23"/>
       <c r="E123"/>
-      <c r="J123" s="248"/>
+      <c r="J123" s="208"/>
       <c r="L123" s="23"/>
       <c r="M123"/>
     </row>
@@ -7724,7 +7854,7 @@
       <c r="B124" s="23"/>
       <c r="D124" s="23"/>
       <c r="E124"/>
-      <c r="J124" s="248"/>
+      <c r="J124" s="208"/>
       <c r="L124" s="23"/>
       <c r="M124"/>
     </row>
@@ -7732,7 +7862,7 @@
       <c r="B125" s="23"/>
       <c r="D125" s="23"/>
       <c r="E125"/>
-      <c r="J125" s="248"/>
+      <c r="J125" s="208"/>
       <c r="L125" s="23"/>
       <c r="M125"/>
     </row>
@@ -7740,7 +7870,7 @@
       <c r="B126" s="23"/>
       <c r="D126" s="23"/>
       <c r="E126"/>
-      <c r="J126" s="248"/>
+      <c r="J126" s="208"/>
       <c r="L126" s="23"/>
       <c r="M126"/>
     </row>
@@ -7748,35 +7878,35 @@
       <c r="B127" s="23"/>
       <c r="D127" s="23"/>
       <c r="E127"/>
-      <c r="J127" s="248"/>
+      <c r="J127" s="208"/>
       <c r="L127" s="23"/>
       <c r="M127"/>
     </row>
     <row r="128" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B128" s="23"/>
-      <c r="J128" s="248"/>
+      <c r="J128" s="208"/>
     </row>
     <row r="129" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B129" s="23"/>
-      <c r="J129" s="248"/>
+      <c r="J129" s="208"/>
     </row>
     <row r="130" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B130" s="23"/>
       <c r="D130" s="23"/>
-      <c r="J130" s="248"/>
+      <c r="J130" s="208"/>
       <c r="L130" s="23"/>
     </row>
     <row r="131" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B131" s="23"/>
-      <c r="J131" s="248"/>
+      <c r="J131" s="208"/>
     </row>
     <row r="132" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B132" s="23"/>
-      <c r="J132" s="248"/>
+      <c r="J132" s="208"/>
     </row>
     <row r="133" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B133" s="23"/>
-      <c r="J133" s="248"/>
+      <c r="J133" s="208"/>
     </row>
     <row r="134" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C134" s="154"/>
@@ -7840,19 +7970,19 @@
   <sheetData>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="43" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="155"/>
-      <c r="B43" s="242" t="s">
-        <v>26</v>
-      </c>
-      <c r="C43" s="243"/>
-      <c r="D43" s="243"/>
-      <c r="E43" s="244"/>
+      <c r="B43" s="272" t="s">
+        <v>25</v>
+      </c>
+      <c r="C43" s="273"/>
+      <c r="D43" s="273"/>
+      <c r="E43" s="274"/>
       <c r="F43" s="1"/>
     </row>
     <row r="44" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7860,16 +7990,16 @@
         <v>44501</v>
       </c>
       <c r="B44" s="157" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C44" s="158">
         <v>484.09</v>
       </c>
       <c r="D44" s="159" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E44" s="160" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F44" s="101">
         <v>333</v>
@@ -7879,16 +8009,16 @@
     <row r="45" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="156"/>
       <c r="B45" s="157" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C45" s="158">
         <v>0</v>
       </c>
       <c r="D45" s="161" t="s">
+        <v>26</v>
+      </c>
+      <c r="E45" s="160" t="s">
         <v>27</v>
-      </c>
-      <c r="E45" s="160" t="s">
-        <v>28</v>
       </c>
       <c r="F45" s="101">
         <v>0</v>
@@ -7898,16 +8028,16 @@
     <row r="46" spans="1:7" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="156"/>
       <c r="B46" s="157" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C46" s="158">
         <v>0</v>
       </c>
       <c r="D46" s="161" t="s">
+        <v>26</v>
+      </c>
+      <c r="E46" s="160" t="s">
         <v>27</v>
-      </c>
-      <c r="E46" s="160" t="s">
-        <v>28</v>
       </c>
       <c r="F46" s="101">
         <v>0</v>
@@ -7916,16 +8046,16 @@
     <row r="47" spans="1:7" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="156"/>
       <c r="B47" s="157" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C47" s="158">
         <v>0</v>
       </c>
       <c r="D47" s="161" t="s">
+        <v>26</v>
+      </c>
+      <c r="E47" s="160" t="s">
         <v>27</v>
-      </c>
-      <c r="E47" s="160" t="s">
-        <v>28</v>
       </c>
       <c r="F47" s="101">
         <v>0</v>
@@ -7934,16 +8064,16 @@
     <row r="48" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="162"/>
       <c r="B48" s="157" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C48" s="158">
         <v>0</v>
       </c>
       <c r="D48" s="163" t="s">
+        <v>26</v>
+      </c>
+      <c r="E48" s="160" t="s">
         <v>27</v>
-      </c>
-      <c r="E48" s="160" t="s">
-        <v>28</v>
       </c>
       <c r="F48" s="101">
         <v>0</v>
@@ -7952,16 +8082,16 @@
     <row r="49" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="162"/>
       <c r="B49" s="157" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C49" s="158">
         <v>0</v>
       </c>
       <c r="D49" s="163" t="s">
+        <v>26</v>
+      </c>
+      <c r="E49" s="160" t="s">
         <v>27</v>
-      </c>
-      <c r="E49" s="160" t="s">
-        <v>28</v>
       </c>
       <c r="F49" s="101">
         <v>0</v>
@@ -7970,16 +8100,16 @@
     <row r="50" spans="1:6" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="162"/>
       <c r="B50" s="157" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C50" s="158">
         <v>0</v>
       </c>
       <c r="D50" s="163" t="s">
+        <v>26</v>
+      </c>
+      <c r="E50" s="160" t="s">
         <v>27</v>
-      </c>
-      <c r="E50" s="160" t="s">
-        <v>28</v>
       </c>
       <c r="F50" s="101">
         <v>0</v>
@@ -7988,16 +8118,16 @@
     <row r="51" spans="1:6" ht="16.5" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="164"/>
       <c r="B51" s="157" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C51" s="158">
         <v>0</v>
       </c>
       <c r="D51" s="165" t="s">
+        <v>26</v>
+      </c>
+      <c r="E51" s="160" t="s">
         <v>27</v>
-      </c>
-      <c r="E51" s="160" t="s">
-        <v>28</v>
       </c>
       <c r="F51" s="101">
         <v>0</v>

</xml_diff>

<commit_message>
CIERRE 19 NOV 2021
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 10  OCTUBRE 2021/BALANCE    ZAVALETA   OCTUBRE   2021.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 10  OCTUBRE 2021/BALANCE    ZAVALETA   OCTUBRE   2021.xlsx
@@ -2081,6 +2081,78 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="56" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="60" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="47" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="6" borderId="51" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="6" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="13" fillId="0" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="50" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2112,78 +2184,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="6" borderId="51" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="6" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="13" fillId="0" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="50" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="43" fillId="6" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2921,7 +2921,7 @@
   </sheetPr>
   <dimension ref="A1:S80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
@@ -2947,23 +2947,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="235"/>
-      <c r="C1" s="237" t="s">
+      <c r="B1" s="259"/>
+      <c r="C1" s="261" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="238"/>
-      <c r="E1" s="238"/>
-      <c r="F1" s="238"/>
-      <c r="G1" s="238"/>
-      <c r="H1" s="238"/>
-      <c r="I1" s="238"/>
-      <c r="J1" s="238"/>
-      <c r="K1" s="238"/>
-      <c r="L1" s="238"/>
-      <c r="M1" s="238"/>
+      <c r="D1" s="262"/>
+      <c r="E1" s="262"/>
+      <c r="F1" s="262"/>
+      <c r="G1" s="262"/>
+      <c r="H1" s="262"/>
+      <c r="I1" s="262"/>
+      <c r="J1" s="262"/>
+      <c r="K1" s="262"/>
+      <c r="L1" s="262"/>
+      <c r="M1" s="262"/>
     </row>
     <row r="2" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="236"/>
+      <c r="B2" s="260"/>
       <c r="C2" s="3"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
@@ -2973,17 +2973,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:19" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="239" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="240"/>
+      <c r="B3" s="263" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="264"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="241" t="s">
+      <c r="H3" s="265" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="241"/>
+      <c r="I3" s="265"/>
       <c r="K3" s="178"/>
       <c r="L3" s="13"/>
       <c r="M3" s="14"/>
@@ -2997,14 +2997,14 @@
         <v>0</v>
       </c>
       <c r="D4" s="18"/>
-      <c r="E4" s="242" t="s">
+      <c r="E4" s="266" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="243"/>
-      <c r="H4" s="244" t="s">
+      <c r="F4" s="267"/>
+      <c r="H4" s="268" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="245"/>
+      <c r="I4" s="269"/>
       <c r="J4" s="19"/>
       <c r="K4" s="179"/>
       <c r="L4" s="20"/>
@@ -3014,10 +3014,10 @@
       <c r="N4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="P4" s="251" t="s">
+      <c r="P4" s="240" t="s">
         <v>6</v>
       </c>
-      <c r="Q4" s="252"/>
+      <c r="Q4" s="241"/>
     </row>
     <row r="5" spans="1:19" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
@@ -4458,11 +4458,11 @@
       <c r="J39" s="60"/>
       <c r="K39" s="190"/>
       <c r="L39" s="61"/>
-      <c r="M39" s="253">
+      <c r="M39" s="242">
         <f>SUM(M5:M38)</f>
         <v>247061</v>
       </c>
-      <c r="N39" s="255">
+      <c r="N39" s="244">
         <f>SUM(N5:N38)</f>
         <v>172863</v>
       </c>
@@ -4488,8 +4488,8 @@
       <c r="J40" s="60"/>
       <c r="K40" s="41"/>
       <c r="L40" s="61"/>
-      <c r="M40" s="254"/>
-      <c r="N40" s="256"/>
+      <c r="M40" s="243"/>
+      <c r="N40" s="245"/>
       <c r="P40" s="34"/>
       <c r="Q40" s="9"/>
     </row>
@@ -4704,29 +4704,29 @@
       <c r="A52" s="98"/>
       <c r="B52" s="99"/>
       <c r="C52" s="1"/>
-      <c r="H52" s="257" t="s">
+      <c r="H52" s="246" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="258"/>
+      <c r="I52" s="247"/>
       <c r="J52" s="100"/>
-      <c r="K52" s="259">
+      <c r="K52" s="248">
         <f>I50+L50</f>
         <v>53873.49</v>
       </c>
-      <c r="L52" s="260"/>
-      <c r="M52" s="261">
+      <c r="L52" s="249"/>
+      <c r="M52" s="250">
         <f>N39+M39</f>
         <v>419924</v>
       </c>
-      <c r="N52" s="262"/>
+      <c r="N52" s="251"/>
       <c r="P52" s="34"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="263" t="s">
+      <c r="D53" s="252" t="s">
         <v>12</v>
       </c>
-      <c r="E53" s="263"/>
+      <c r="E53" s="252"/>
       <c r="F53" s="101">
         <f>F50-K52-C50</f>
         <v>471038.61</v>
@@ -4737,22 +4737,22 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="263" t="s">
+      <c r="D54" s="252" t="s">
         <v>101</v>
       </c>
-      <c r="E54" s="263"/>
+      <c r="E54" s="252"/>
       <c r="F54" s="96">
         <v>-549976.4</v>
       </c>
-      <c r="I54" s="264" t="s">
+      <c r="I54" s="253" t="s">
         <v>13</v>
       </c>
-      <c r="J54" s="265"/>
-      <c r="K54" s="266">
+      <c r="J54" s="254"/>
+      <c r="K54" s="255">
         <f>F56+F57+F58</f>
         <v>-24577.400000000023</v>
       </c>
-      <c r="L54" s="267"/>
+      <c r="L54" s="256"/>
       <c r="P54" s="34"/>
       <c r="Q54" s="9"/>
     </row>
@@ -4785,11 +4785,11 @@
         <v>15</v>
       </c>
       <c r="J56" s="109"/>
-      <c r="K56" s="268">
+      <c r="K56" s="257">
         <f>-C4</f>
         <v>0</v>
       </c>
-      <c r="L56" s="269"/>
+      <c r="L56" s="258"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="110" t="s">
@@ -4806,22 +4806,22 @@
       <c r="C58" s="112">
         <v>44507</v>
       </c>
-      <c r="D58" s="246" t="s">
+      <c r="D58" s="235" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="247"/>
+      <c r="E58" s="236"/>
       <c r="F58" s="113">
         <v>567389.35</v>
       </c>
-      <c r="I58" s="248" t="s">
+      <c r="I58" s="237" t="s">
         <v>103</v>
       </c>
-      <c r="J58" s="249"/>
-      <c r="K58" s="250">
+      <c r="J58" s="238"/>
+      <c r="K58" s="239">
         <f>K54+K56</f>
         <v>-24577.400000000023</v>
       </c>
-      <c r="L58" s="250"/>
+      <c r="L58" s="239"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="114"/>
@@ -4965,6 +4965,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:M1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="D58:E58"/>
     <mergeCell ref="I58:J58"/>
     <mergeCell ref="K58:L58"/>
@@ -4979,12 +4985,6 @@
     <mergeCell ref="I54:J54"/>
     <mergeCell ref="K54:L54"/>
     <mergeCell ref="K56:L56"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:M1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.15748031496062992" top="0.35433070866141736" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="75" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>